<commit_message>
Test commit, added tes log message
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ytymkiv001\Documents\Robots\orchestratorJobsTime\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F5A3B7-8C07-4A15-B950-EF2CEDB158B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53111B48-FC0F-4BF1-9032-69CED2917F4F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>orchestratorURL</t>
   </si>
   <si>
-    <t>https://gz-zwewebdwv267.cee.ema.ad.pwcinternal.com/</t>
-  </si>
-  <si>
     <t>Orchestrator's URL</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>Login credentials</t>
+  </si>
+  <si>
+    <t>https://orchestrator.com/</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -616,13 +616,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -631,109 +631,109 @@
         <v>25</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="5">
         <v>43832</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Reworked process of filtering jobs.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ytymkiv001\Documents\Robots\orchestratorJobsTime\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3486BA50-553A-4358-80F6-718CF669D334}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FA10DA-5D6B-49E9-BE9D-A91A75FA96D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -145,21 +145,9 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>03/15/2020</t>
-  </si>
-  <si>
-    <t>GetTimeInBucharest_Test,BlankProcess_Tost</t>
-  </si>
-  <si>
     <t>List of jobs that robot will collect. Comma (,) is delimiter.</t>
   </si>
   <si>
-    <t>First date of range</t>
-  </si>
-  <si>
-    <t>Last date of range</t>
-  </si>
-  <si>
     <t>Difference in time zones. Robot will shift output times on that value. Positive and negative numbers allowed</t>
   </si>
   <si>
@@ -169,16 +157,31 @@
     <t>0 - CSV, 1 - XLSX</t>
   </si>
   <si>
+    <t>Login credentials</t>
+  </si>
+  <si>
+    <t>2020-01-01</t>
+  </si>
+  <si>
+    <t>2020-03-31</t>
+  </si>
+  <si>
+    <t>Last date of range. Format: yyyy-mm-dd</t>
+  </si>
+  <si>
+    <t>First date of range. Format: yyyy-mm-dd</t>
+  </si>
+  <si>
+    <t>GetTimeInBucharest_Test</t>
+  </si>
+  <si>
+    <t>https://orchestartor.com/</t>
+  </si>
+  <si>
     <t>username</t>
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>Login credentials</t>
-  </si>
-  <si>
-    <t>https://orchestrator.com/</t>
   </si>
 </sst>
 </file>
@@ -244,12 +247,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -568,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -621,7 +624,7 @@
       <c r="B2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -630,8 +633,8 @@
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>51</v>
+      <c r="B4" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>26</v>
@@ -657,7 +660,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -665,7 +668,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -674,7 +677,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -683,22 +686,22 @@
       <c r="A11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="5">
-        <v>43832</v>
+      <c r="B11" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>40</v>
+      <c r="B12" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -707,22 +710,22 @@
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
@@ -733,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1719,7 +1722,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{C47C391F-CB7D-4BF6-B518-A01ABEBF7B88}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{EA885FE4-B6FC-4C9C-A31E-DC3626B0E000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>